<commit_message>
rut gon ten camera
</commit_message>
<xml_diff>
--- a/pre-processing/data_cleaned/camera.xlsx
+++ b/pre-processing/data_cleaned/camera.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +531,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>bo chuyen đoi nguon đien 220v sang 12v cong ra tau đien tren o to</t>
+          <t>bo chuyen nguon 220v sang 12v o to</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -571,7 +571,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>camera wifi yoosee ngoai troi 20mpx 4 mat 3 man hinh kep q10-28 phien ban moi 2025,đem co mau, đam thoai hai chieu, chong nuoc nhua ip66, hang nhap khau</t>
+          <t>camera yoosee ngoai troi q10-28 20mpx</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>camera yoosee wifi ngoai troi 2 mat xem cung luc, goc rong, đam thoai, ip66 chong nuoc, bao đong, hang nhap khau - bao hanh 12 thang</t>
+          <t>camera yoosee ngoai troi 2 mat</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>pin danh cho may anh nikon en-el14 1500mah cao cap - hang nhap khau</t>
+          <t>pin may anh nikon en-el14</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>the vietmap live pro chinh hang 2025, canh bao toc đo, camera phat nguoi dung tren đien thoai, android.box, man hinh o to - hang chinh hang</t>
+          <t>the vietmap live pro 2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -731,7 +731,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>camera hanh trinh 70mai m310 ghi hinh 2k (qhd) goc quay rong 130° (cam truoc) - hang chinh hang</t>
+          <t>camera hanh trinh 70mai m310 2k</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>camera ip wifi ezviz c6n pro 2k (3mp) - phien ban nang cap cua c6n - hang chinh hang</t>
+          <t>camera ezviz c6n pro 2k 3mp</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>camera wifi ezviz ngoai troi h8c pro 3mp phat hien chuyen đong, quay 360, đam thoai 2 chieu- hang chinh hang</t>
+          <t>camera ezviz ngoai troi h8c pro 3mp</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -851,7 +851,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>bo day đeo nguc 5 chi tiet cho may quay hanh đong, smartphone 077, hang chinh hang</t>
+          <t>bo day đeo nguc cho may quay</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>camera wifi ngoai troi tp-link tapo c520ws - đo phan giai 2k 4mp, chong chiu thoi tiet ip66, co mau ban đem - hang chinh hang</t>
+          <t>camera tp-link tapo c520ws 2k 4mp</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>the nho 32gb/ 64gb sdhc/ sdxc lexar 800x pro uhs-i blue series, toc đo đoc len đen 150mb/s - hang chinh hang</t>
+          <t>the nho lexar 800x pro 32gb/64gb</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>camera ip wifi trong nha ezviz c6n 1080p - hang chinh hang</t>
+          <t>camera ezviz c6n 1080p</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>camera ip trong nha tapo c212 - quay quet 360, đo phan giai 2k 3mp, đam thoai 2 chieu, co hong ngoai ban đem - hang chinh hang</t>
+          <t>camera tapo c212 2k 3mp</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>camera wifi ezviz 2 mat trong nha h7c 2k 8mp, quay 360 đo, co mau ban đem, đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera ezviz 2 mat h7c 2k 8mp</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>camera wifi ezviz 2 mat ngoai troi h9c 3k 6mp/10mp, quay 360 đo, đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera ezviz 2 mat ngoai troi h9c 3k</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(mau moi) camera yoosee bong đen 2 mat qs211 fhd xem 2 khung hinh, hinh anh sac net, quay đem co mau - hang chinh hang</t>
+          <t>camera yoosee bong đen qs211 fhd</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>camera wifi tp-link tapo c510w / c520ws an ninh quay/quet 360 đo, chong nuoc - hang chinh hang</t>
+          <t>camera tp-link tapo c510w / c520ws</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>camera wifi ezviz h3c 2mp co mau ban đem, h3c 1080p mic thu am - hang chinh hang</t>
+          <t>camera ezviz h3c 2mp</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>(mau 2024) camera 4g yoosee 2 mat xem 2 man hinh 5.0mpx xoay 360 đo, xem đem co mau, ho tro đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera 4g yoosee 2 mat 5.0mpx</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>camera yoosee wifi 2 mat ngoai troi 2 man hinh 5mp xem đem co mau, ho tro đam thoai 2 chieu xoay 360 đo - hang nhap khau</t>
+          <t>camera yoosee wifi ngoai troi 2 mat 5mp</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>camera wifi yoosee 2 mat ngoai troi, xem 2 man hinh cung luc, giam sat ngoai troi chong nuoc ip66 - hang nhap khau</t>
+          <t>camera yoosee 2 mat ngoai troi (chong nuoc)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>camera yoosee 2 mat trong nha 4mp ket noi wifi, xoay 360 đo, đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera yoosee 2 mat trong nha 4mp</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>camera wifi trong nha quay quet 3mp imou ipc-a32ep-l - hang chinh hang</t>
+          <t>camera imou ipc-a32ep-l 3mp</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>camera wifi tp-link tapo c510w an ninh quay/quet 360 đo, chong nuoc - hang chinh hang</t>
+          <t>camera tp-link tapo c510w</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>camera wifi yoosee 2 mat xem 2 man hinh cung luc ngoai troi - hang nhap khau</t>
+          <t>camera yoosee 2 mat ngoai troi</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>camera wifi imou a22ep 1080p xoay 360 đo - đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera imou a22ep 1080p</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>camera ip wifi quay quet thong minh ezviz c6n 2.0 4.0mp - hang chinh hang</t>
+          <t>camera ezviz c6n 4.0mp</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>camera co mau ban đem ip hong ngoai khong day 2.0 3.0 megapixel ezviz c3tn  - hang chinh hang</t>
+          <t>camera ezviz c3tn 3.0mp</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>camera imou cue 2, camera wifi đo phan giai 2 megapixel, đam thoai 2 chieu, phat hien nguoi bang ai thong minh - hang chinh hang</t>
+          <t>camera imou cue 2 2mp</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>camera wifi ngoai troi tp-link tapo c320ws đo phan giai 2k qhd - hang chinh hang</t>
+          <t>camera tp-link tapo c320ws 2k</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>camera ip wifi imou ranger a2 full hd 1080p, phien ban 2022 - hang chinh hang</t>
+          <t>camera imou ranger a2 1080p</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>the nho 32/64/128/256gb mixie  microsd  class10 u3. hang chinh hang</t>
+          <t>the nho mixie microsd class10 u3</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>bo chuyen nguon poe 48v-12v dung cho camera, hang chinh hang</t>
+          <t>bo chuyen nguon poe 48v-12v</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1851,7 +1851,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>đau đoc the nho ssk cho may anh - hang chinh hang</t>
+          <t>đau đoc the nho ssk cho may anh</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>pin panasonic cr 1632 -hang chinh hang</t>
+          <t>pin panasonic cr 1632</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>camera wifi yoosee 3.0  2k sieu net - camera ip yoosee 3 rau 3mp trong nha - hang nhap khau</t>
+          <t>camera yoosee 3 rau 3mp 2k</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>camera wi-fi tp-link tapo c200 1080p (2mp) an ninh gia đinh co the đieu chinh huong - hang chinh hang</t>
+          <t>camera tp-link tapo c200 1080p</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>goi hut am secco - hang chinh hang</t>
+          <t>goi hut am secco</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>goi hut am đa dung loai 2gr - 100g - hang chinh hang</t>
+          <t>goi hut am đa dung 2g - 100g</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>balo may anh, balo camera chong nuoc natoli, nhieu ngan đung laptop đi du lich chinh hang bst durable premium camera backpack b29</t>
+          <t>balo may anh natoli chong nuoc</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>camera hanh trinh vietmap ts-c9p - hang chinh hang</t>
+          <t>camera hanh trinh vietmap ts-c9p</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>camera quan sat xiaomi c400 smart 2.5k - hang nhap khau</t>
+          <t>camera xiaomi c400 2.5k</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2211,7 +2211,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>chan đe camera, gia đo camera dan tuong trong suot - hang chinh hang</t>
+          <t>chan đe camera dan tuong</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>nguon adapter 12v 2a; 3a; 5a; 6a cho đen led, camera - hang chinh hang - 12v2a 24w</t>
+          <t>nguon adapter 12v</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>the nho sd sandisk ultra gn3 32gb 100mb/s uhs-i (cho may anh) - hang chinh hang</t>
+          <t>the nho sd sandisk 32gb cho may anh</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>camera nang luong mat troi 4g khong day netcam stl4g, chat luong video hd 4mp, dung sim 4g, dung luong pin 8000mah - hang chinh hang</t>
+          <t>camera nang luong mat troi netcam stl4g 4g</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2371,7 +2371,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1 kg goi hut am 5/10/20gr nhan hieu maxdesi hang chinh hang</t>
+          <t>1kg goi hut am maxdesi</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>camera ip wifi quay quet ngoai troi ezviz h8c 4mp 2k+ - hang chinh hang</t>
+          <t>camera ezviz h8c 4mp 2k+</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2451,7 +2451,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>godox sl100d / sl100bi - đen led ho tro cho quay phim, chup hinh, đieu khien app, cong suat toi đa 100w - hang chinh hang</t>
+          <t>đen led godox sl100d / sl100bi</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>camera wifi imou 2 mat ngoai troi s7xp cruiser dual 6mp/10mp, quay 360 đo, đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera imou 2 mat s7xp cruiser dual</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2531,7 +2531,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>camera wifi tp-link tapo c211 đo phan giai 2k uhd quay quet 360 đo - hang chinh hang</t>
+          <t>camera tp-link tapo c211 2k</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2571,7 +2571,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[[mau nang cap] camera wi-fi ezviz h1c/c1hc trong nha, fhd 1080p, goc rong co đinh, đam thoai hai chieu, nen video h265 - hang chinh hang</t>
+          <t>camera ezviz h1c/c1hc 1080p</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2611,7 +2611,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>camera wifi ezviz cs-h1c (2.0mp) - hang chinh hang</t>
+          <t>camera ezviz cs-h1c 2.0mp</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>camera yoosee wifi 2 mat ngoai troi qpt36 xem 2 man hinh cung luc 5.0mpx giam sat ngoai troi chong nuoc ip66 - hang chinh hang</t>
+          <t>camera yoosee 2 mat ngoai troi qpt36 5.0mpx</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2691,7 +2691,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>camera ip yoosee ptz ngoai troi 2 man hinh 5mpx xem đem co mau, ho tro đam thoai 2 chieu xoay 360 đo - hang chinh hang</t>
+          <t>camera yoosee ptz ngoai troi 2 mat 5mpx</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2731,7 +2731,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>camera yoosee wifi 2 mat sieu net - xem 2 man hinh cung luc - hang chinh hang</t>
+          <t>camera yoosee wifi 2 mat</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2771,7 +2771,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>flycam zll sg108 max tich hop cam bien laser tranh vat can thong minh - thiet bi bay co song wifi 5g the he moi - hang nhap khau</t>
+          <t>flycam zll sg108 max</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2811,7 +2811,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>camera giam sat chong trom, camera wifi mini khong day a9, đo phan giai 720p, app xem tu xa - hang chinh hang miniin</t>
+          <t>camera mini a9 720p</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>hohem isteady xe / xe kit - gimbal chong rung cho smartphone, tai trong 280g, su dung 8 gio- hang chinh hang</t>
+          <t>gimbal hohem isteady xe / xe kit</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2891,7 +2891,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>camera ip wifi imou ranger 2 ipc - a22ep full hd 1080p - hang chinh hang</t>
+          <t>camera imou ranger 2 ipc-a22ep 1080p</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2931,7 +2931,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>camera yoosee pt nang luong mat troi cg19-46 (solar pt camera 4.0mpx) - hang chinh hang</t>
+          <t>camera yoosee nang luong mat troi cg19-46</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>camera wifi ezviz h8 3k - đo phan giai 5mp, bao phu toan canh 360 đo, phat hien con nguoi, đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera ezviz h8 3k 5mp</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1 kg goi hut am loai 10gr (100 goi) nhan hieu max desi hang chinh hang</t>
+          <t>1kg goi hut am max desi 10gr</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3051,7 +3051,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>camera ip wifi trong nha ezviz c6n 4m 2k, xoay 360 đo ezviz c6n full hd, đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera ezviz c6n 4m 2k</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>camera ip wifi ngoai troi ezviz h8 3k 5mp - hang chinh hang</t>
+          <t>camera ezviz h8 ngoai troi 3k 5mp</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3131,7 +3131,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>camera imou cruiser 2mp/4mp, camera ngoai troi, xoay 360, chong nuoc, tich hop đen chieu sang, co mau ban đem - hang chinh hang</t>
+          <t>camera imou cruiser 2mp/4mp</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3171,7 +3171,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>camera ip wifi ngoai troi ezviz h3 5mp đo phan giai 3k sieu net tich hop ai nhan dien vay tay chao - co mau ban đem - đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera ezviz h3 5mp 3k</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3211,7 +3211,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>camera ip wifi ngoai troi ezviz c3tn 3mp 2k color night vision tich hop ai - co mau ban đem - đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera ezviz c3tn 3mp 2k</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3251,7 +3251,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>camera wifi trong nha ezviz c6n 2m fhd 1080p quay 355 đo - đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera ezviz c6n 2m 1080p</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3291,7 +3291,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>camera wifi ngoai troi tp-link tapo c320ws 4mp - hang chinh hang</t>
+          <t>camera tp-link tapo c320ws 4mp</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>the nho sdhc sandisk ultra 16gb upto 80mb/s uhs-i (cho may anh) - hang chinh hang</t>
+          <t>the nho sdhc sandisk 16gb cho may anh</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>camera ip wifi trong nha imou ranger 2 2mp/4mp - hang chinh hang</t>
+          <t>camera imou ranger 2 2mp/4mp</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3411,7 +3411,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>camera imou range 2c - new 2021 - chip hinh anh the he moi - wifi cuc manh sieu khoe - hang chinh hang</t>
+          <t>camera imou range 2c</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>camera ip 360 đo 1080p tp-link tapo c200 trang - hang chinh hang</t>
+          <t>camera tp-link tapo c200 1080p</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3491,7 +3491,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>combo camera wi-fi trong nha ezviz c1c-b 2mp kem the nho  32gb/64g - hang chinh hang</t>
+          <t>combo camera ezviz c1c-b 2mp + the nho</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3531,7 +3531,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>tripod - chan đe đien thoai, chan đe may anh yunteng vct 5208 kiem gia đo co remote bluetooth đieu khien chup tu xa</t>
+          <t>tripod yunteng vct 5208</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>camera wifi trong nha yoosee 3.0 full hd, 3 rau, xoay 360 đo , đam thoai 2 chieu, cam bien bao đong – hang nhap khau</t>
+          <t>camera yoosee trong nha 3.0 fhd 3 rau</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3611,7 +3611,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>camera ip wifi ezviz cs - c1c - 2mp</t>
+          <t>camera ezviz cs-c1c 2mp</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>camera ip wifi trong nha ezviz c6n 1080p - hang chinh hang</t>
+          <t>camera ezviz c6n 1080p</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3691,7 +3691,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>may chup anh mini kem the 512g t retro ky thuat so ccd 4k cho hoc sinh – nho gon, thoi trang, chup sieu net- hang chinh hang miniin</t>
+          <t>may anh mini retro ky thuat so 4k</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3731,7 +3731,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>bo nap van bao ap suat lop o to, xe may</t>
+          <t>bo nap van bao ap suat lop</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3771,7 +3771,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>camera hanh trinh o to đo phan giai 2k, wifi, uhd thuong hieu hp f965s - hang chinh hang</t>
+          <t>camera hanh trinh hp f965s 2k</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3811,7 +3811,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>ulanzi mt-79 / mt-89 - tripod đa nang cho may anh, đien thoai, thiet bi chieu sang, chieu cao đa dang - hang chinh hang</t>
+          <t>tripod ulanzi mt-79 / mt-89</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>camera wifi quay quet ezviz h6c pro 3k 5mp - hang chinh hang</t>
+          <t>camera ezviz h6c pro 3k 5mp</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3891,7 +3891,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>camera noi soi cong nghiep chong nuoc ket noi đien thoai an112 - hang nhap khau</t>
+          <t>camera noi soi an112</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3931,7 +3931,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>camera hanh trinh sjcam c110 plus ban 2024 - actioncam c110+ 4k wifi chong rung kep camera mini - hang nhap khau</t>
+          <t>camera hanh trinh sjcam c110 plus 4k</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3971,7 +3971,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>camera ip 360 đo 2mp tp-link tapo tc70 - hang chinh hang</t>
+          <t>camera tp-link tapo tc70 2mp</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -4007,131 +4007,131 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>275511061</v>
+        <v>275326681</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>may do camera an xm smoovie chong quay len va canh bao chong trom - thiet bi do hong ngoai phat hien chuyen đong - hang chinh hang</t>
+          <t>camera noi soi rogtz p10</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>xm</t>
+          <t>rogtz</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>images/camera/product_275511061.jpg</t>
+          <t>images/camera/product_275326681.jpg</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/4a/88/d8/32e76c61214443bc2a1bce128a0f4075.jpg</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/d6/d7/1c/742430ccfe1d0e3113d38dd7fb0cd44b.jpg</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>298920</v>
+        <v>858000</v>
       </c>
       <c r="G90" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H90" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I90" t="n">
-        <v>275511070</v>
+        <v>275326687</v>
       </c>
       <c r="J90" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>275326681</v>
+        <v>274847176</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>rogtz - camera noi soi p10 chong nuoc ip68 man hinh ips 2.8 inch đuong kinh camera 3.9mm đo phan giai cao 1080p 8 đen led đa ngon ngu  pin lithium dung luong cao 3.7v 2600mah nha xuong y te cam tay o to nha cua hang chinh hang</t>
+          <t>camera ngoai troi netcam std34 6mp</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>rogtz</t>
+          <t>netcam</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>images/camera/product_275326681.jpg</t>
+          <t>images/camera/product_274847176.jpg</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/d6/d7/1c/742430ccfe1d0e3113d38dd7fb0cd44b.jpg</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/52/32/04/7dac33f95e51ae89f9f88181337fa87f.jpg</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>858000</v>
+        <v>729000</v>
       </c>
       <c r="G91" t="n">
         <v>4</v>
       </c>
       <c r="H91" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I91" t="n">
-        <v>275326687</v>
+        <v>274847178</v>
       </c>
       <c r="J91" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>274847176</v>
+        <v>274179036</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>camera ngoai troi netcam std34, quay quet 360 đo, co ong kinh kep voi đo phan giai sieu net 6mp - hang chinh hang</t>
+          <t>camera yoosee r3 3 mat 8.0mpx</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>netcam</t>
+          <t>yoosee</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>images/camera/product_274847176.jpg</t>
+          <t>images/camera/product_274179036.jpg</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/52/32/04/7dac33f95e51ae89f9f88181337fa87f.jpg</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/c6/6e/08/358ecfb3a456ea83fabe958dd0539818.jpg</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>729000</v>
+        <v>644000</v>
       </c>
       <c r="G92" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H92" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I92" t="n">
-        <v>274847178</v>
+        <v>274179038</v>
       </c>
       <c r="J92" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>274179036</v>
+        <v>273474185</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>camera ip wifi yoosee r3 co 3 mat ngoai troi xem 3 man hinh cung luc, đo phan giai 8.0mpx - hang chinh hang</t>
+          <t>camera yoosee ptz 2 mat</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -4141,277 +4141,277 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>images/camera/product_274179036.jpg</t>
+          <t>images/camera/product_273474185.jpg</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/c6/6e/08/358ecfb3a456ea83fabe958dd0539818.jpg</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/d2/5e/7e/3146ff5bb31829008fc6ca0834208d9c.jpg</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>644000</v>
+        <v>375250</v>
       </c>
       <c r="G93" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H93" t="n">
         <v>4.5</v>
       </c>
       <c r="I93" t="n">
-        <v>274179038</v>
+        <v>270977296</v>
       </c>
       <c r="J93" t="n">
-        <v>10</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>273474185</v>
+        <v>273446601</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>camera wifi yoosee ptz 2 mat xoay 360 đo - đam thoai 2 chieu - bao đong chong trom - ban đem co mau - hang nhap khau</t>
+          <t>bo ve sinh ong kinh may anh kai.n</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>yoosee</t>
+          <t>kai nguyen</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>images/camera/product_273474185.jpg</t>
+          <t>images/camera/product_273446601.jpg</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/d2/5e/7e/3146ff5bb31829008fc6ca0834208d9c.jpg</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/c5/0b/0b/e096c3f0c5051f015b25b168d8afbaea.png</t>
         </is>
       </c>
       <c r="F94" t="n">
-        <v>375250</v>
+        <v>59000</v>
       </c>
       <c r="G94" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H94" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="I94" t="n">
-        <v>270977296</v>
+        <v>273446602</v>
       </c>
       <c r="J94" t="n">
-        <v>117</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>273446601</v>
+        <v>273026293</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>bo dung dich dung cu ve sinh kai.n cleaning sulution danh cho iphone, ipad, laptop, ong kinh may anh, thiet bi khac - hang chinh hang</t>
+          <t>camera hanh trinh s10 plus 3 mat</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>kai nguyen</t>
+          <t>viethas</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>images/camera/product_273446601.jpg</t>
+          <t>images/camera/product_273026293.jpg</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/c5/0b/0b/e096c3f0c5051f015b25b168d8afbaea.png</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/21/dd/06/810c1b49b44da03886128e96ff2e7e96.jpg</t>
         </is>
       </c>
       <c r="F95" t="n">
-        <v>59000</v>
+        <v>760000</v>
       </c>
       <c r="G95" t="n">
+        <v>13</v>
+      </c>
+      <c r="H95" t="n">
         <v>0</v>
       </c>
-      <c r="H95" t="n">
-        <v>5</v>
-      </c>
       <c r="I95" t="n">
-        <v>273446602</v>
+        <v>273026297</v>
       </c>
       <c r="J95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>273026293</v>
+        <v>272178556</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>camera hanh trinh o to 3 mat s10 plus co wifi full hd 1080p ho tro ket noi đien thoai xem qua app - hang chinh hang</t>
+          <t>camera ezviz h6 5mp 3k</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>viethas</t>
+          <t>ezviz</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>images/camera/product_273026293.jpg</t>
+          <t>images/camera/product_272178556.jpg</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/21/dd/06/810c1b49b44da03886128e96ff2e7e96.jpg</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/a2/be/00/d11ffdda4e333befcb4fc65fe03cd1c1.png</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>760000</v>
+        <v>837000</v>
       </c>
       <c r="G96" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H96" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I96" t="n">
-        <v>273026297</v>
+        <v>272178558</v>
       </c>
       <c r="J96" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>272178556</v>
+        <v>271705499</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>camera wifi ai thong minh ezviz h6 5mp 3k sieu net, xoay 360 đo, đam thoai 2 chieu - hang chinh hang</t>
+          <t>camera tp-link tapo c212 2k</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>ezviz</t>
+          <t>tp link</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>images/camera/product_272178556.jpg</t>
+          <t>images/camera/product_271705499.jpg</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/a2/be/00/d11ffdda4e333befcb4fc65fe03cd1c1.png</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/b8/10/9b/f8c1cbd37f2a6c255e604d8a2367991e.jpg</t>
         </is>
       </c>
       <c r="F97" t="n">
-        <v>837000</v>
+        <v>379000</v>
       </c>
       <c r="G97" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="H97" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="I97" t="n">
-        <v>272178558</v>
+        <v>273290126</v>
       </c>
       <c r="J97" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>271705499</v>
+        <v>271248861</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>camera wifi tp-link tapo c212 đo phan giai 2k qhd quay/quet 360 đo ho tro cong lan - hang chinh hang</t>
+          <t>camera yoosee 2 mat q26d 6x zoom</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>tp link</t>
+          <t>viethas</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>images/camera/product_271705499.jpg</t>
+          <t>images/camera/product_271248861.jpg</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/b8/10/9b/f8c1cbd37f2a6c255e604d8a2367991e.jpg</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/9c/5a/0f/de1d8feaf18c9d86dc37020a1d988c5b.jpg</t>
         </is>
       </c>
       <c r="F98" t="n">
-        <v>379000</v>
+        <v>509000</v>
       </c>
       <c r="G98" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H98" t="n">
-        <v>4.7</v>
+        <v>4</v>
       </c>
       <c r="I98" t="n">
-        <v>273290126</v>
+        <v>276920103</v>
       </c>
       <c r="J98" t="n">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>271248861</v>
+        <v>270906792</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>camera yoosee 2 mat q26d phien ban phong to 6x cuc net - camera kep xem cung luc tren đien thoai, đam thoai 2 chieu, ban đem co mau - hang chinh hang</t>
+          <t>camera tp-link tapo c220 2k</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>viethas</t>
+          <t>tp link</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>images/camera/product_271248861.jpg</t>
+          <t>images/camera/product_270906792.jpg</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/9c/5a/0f/de1d8feaf18c9d86dc37020a1d988c5b.jpg</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/c5/1c/d7/18cbb0ab6202da51d81f1593cb0469c7.jpg</t>
         </is>
       </c>
       <c r="F99" t="n">
-        <v>509000</v>
+        <v>450000</v>
       </c>
       <c r="G99" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H99" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I99" t="n">
-        <v>276920103</v>
+        <v>278050464</v>
       </c>
       <c r="J99" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>270906792</v>
+        <v>263987622</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>camera wifi tp-link tapo c220 đo phan giai 2k qhd quay/quet 360 đo giam sat an ninh - hang chinh hang</t>
+          <t>camera tp-link tapo c200 / c210 1080p</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4421,67 +4421,27 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>images/camera/product_270906792.jpg</t>
+          <t>images/camera/product_263987622.jpg</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/c5/1c/d7/18cbb0ab6202da51d81f1593cb0469c7.jpg</t>
+          <t>https://salt.tikicdn.com/cache/280x280/ts/product/89/28/d3/5dddbd6b7bede5f2947f40de6fa949d2.jpg</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>450000</v>
+        <v>296100</v>
       </c>
       <c r="G100" t="n">
-        <v>13</v>
+        <v>6.5</v>
       </c>
       <c r="H100" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I100" t="n">
-        <v>278050464</v>
+        <v>272042494</v>
       </c>
       <c r="J100" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>263987622</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>camera wifi tp-link tapo c200 / c210 smart ir full hd 1080p - hang chinh hang</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>tp link</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>images/camera/product_263987622.jpg</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>https://salt.tikicdn.com/cache/280x280/ts/product/89/28/d3/5dddbd6b7bede5f2947f40de6fa949d2.jpg</t>
-        </is>
-      </c>
-      <c r="F101" t="n">
-        <v>296100</v>
-      </c>
-      <c r="G101" t="n">
-        <v>11</v>
-      </c>
-      <c r="H101" t="n">
-        <v>4</v>
-      </c>
-      <c r="I101" t="n">
-        <v>272042494</v>
-      </c>
-      <c r="J101" t="n">
         <v>14</v>
       </c>
     </row>

</xml_diff>